<commit_message>
How many opn jobs
</commit_message>
<xml_diff>
--- a/TestData/loginData.xlsx
+++ b/TestData/loginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madhur.Sakharwade\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Madhur.Sakharwade\PycharmProjects\pythonProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDC2466-609A-4399-9BBC-D9F332A05F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23F38DE-666F-4F0B-A905-D2073DFB72EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ED5FFA20-0668-4F93-AB08-6462D5EB39D9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -54,21 +54,6 @@
   </si>
   <si>
     <t>pass</t>
-  </si>
-  <si>
-    <t>dm11163</t>
-  </si>
-  <si>
-    <t>vishal.saha@demo.com</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>DM11163</t>
-  </si>
-  <si>
-    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -454,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46563507-57E0-490E-8A20-0F11EBF91D82}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,43 +473,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{CF35CB7A-D03E-4524-ADCA-346093163E2B}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{9612FD62-39CE-4D62-A5CA-6FEA9A48B95B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>